<commit_message>
changes to SLAReport, AReport, SLASlicer, and added MARsReport
</commit_message>
<xml_diff>
--- a/automated_sla_tool/settings/misterp_settings.xlsx
+++ b/automated_sla_tool/settings/misterp_settings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mscales\Desktop\Development\automated_sla_tool\program_files\settings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mscales\Desktop\Development\automated_sla_tool\automated_sla_tool\settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Constant</t>
   </si>
@@ -44,40 +44,7 @@
     <t>SETTINGS_PIC</t>
   </si>
   <si>
-    <t>CALL_SLA_ARG</t>
-  </si>
-  <si>
-    <t>ACCUM_ARG</t>
-  </si>
-  <si>
-    <t>SPREADSHEET_VIEWER_FILE_TEMPLATE</t>
-  </si>
-  <si>
-    <t>ACCUM_VIEWER_FILE</t>
-  </si>
-  <si>
-    <t>TEST_SPREADSHEET</t>
-  </si>
-  <si>
     <t>ACCUM_PIC</t>
-  </si>
-  <si>
-    <t>C:\users\mscales\desktop\development\daily sla parser - automated version\bin\cli.py</t>
-  </si>
-  <si>
-    <t>C:\users\mscales\desktop\development\MSSQLupdater\bin\client_counter.py</t>
-  </si>
-  <si>
-    <t>C:\users\\mscales\desktop\Development\Daily SLA Parser - Automated Version\Output\{0}v2_Incoming DID Summary.xlsx</t>
-  </si>
-  <si>
-    <t>C:\users\mscales\desktop\development\MSSQLupdater\output\temp_file.xlsx</t>
-  </si>
-  <si>
-    <t>CALL_SLICER_ARG</t>
-  </si>
-  <si>
-    <t>C:\Users\mscales\Desktop\Development\automated_sla_tool\program_files\bin\sla_slicer.py</t>
   </si>
   <si>
     <t>go.png</t>
@@ -444,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,15 +436,15 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -485,7 +452,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -493,7 +460,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -501,55 +468,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>